<commit_message>
rem to loc from PI
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Smith\Desktop\MiTech Backup\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29F3A5F-8D64-4840-8068-442536232BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277CC6E0-07AC-4A4D-853E-BED150B6E5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4090" yWindow="1930" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Power While Running</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>M_full_half_png_Remote_to_PI</t>
+  </si>
+  <si>
+    <t>M_full_png_remote_to_local_from_PI</t>
   </si>
 </sst>
 </file>
@@ -397,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" customWidth="1"/>
     <col min="4" max="4" width="13.1796875" customWidth="1"/>
   </cols>
@@ -442,106 +445,121 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>3.1025999999999998</v>
+        <v>2.8386999999999998</v>
       </c>
       <c r="C3">
-        <v>2.9518</v>
+        <v>2.7683</v>
       </c>
       <c r="D3">
         <f xml:space="preserve"> B3 - C3</f>
-        <v>0.15079999999999982</v>
+        <v>7.0399999999999796E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>3.0836000000000001</v>
+        <v>3.1025999999999998</v>
       </c>
       <c r="C4">
-        <v>2.9333</v>
+        <v>2.9518</v>
       </c>
       <c r="D4">
-        <f xml:space="preserve"> B4 - C4</f>
-        <v>0.1503000000000001</v>
+        <f t="shared" ref="D4:D10" si="0" xml:space="preserve"> B4 - C4</f>
+        <v>0.15079999999999982</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>3.0442</v>
+        <v>3.0836000000000001</v>
       </c>
       <c r="C5">
-        <v>2.91</v>
+        <v>2.9333</v>
       </c>
       <c r="D5">
-        <f xml:space="preserve"> B5 - C5</f>
-        <v>0.13419999999999987</v>
+        <f t="shared" si="0"/>
+        <v>0.1503000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>3.0968</v>
+        <v>3.0442</v>
       </c>
       <c r="C6">
-        <v>2.9352</v>
+        <v>2.91</v>
       </c>
       <c r="D6">
-        <f xml:space="preserve"> B6 - C6</f>
-        <v>0.16159999999999997</v>
+        <f t="shared" si="0"/>
+        <v>0.13419999999999987</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>3.0960000000000001</v>
+        <v>3.0968</v>
       </c>
       <c r="C7">
-        <v>2.9740000000000002</v>
+        <v>2.9352</v>
       </c>
       <c r="D7">
-        <f xml:space="preserve"> B7 - C7</f>
-        <v>0.12199999999999989</v>
+        <f t="shared" si="0"/>
+        <v>0.16159999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>3.0981000000000001</v>
+        <v>3.0960000000000001</v>
       </c>
       <c r="C8">
-        <v>2.9417</v>
+        <v>2.9740000000000002</v>
       </c>
       <c r="D8">
-        <f xml:space="preserve"> B8 - C8</f>
-        <v>0.15640000000000009</v>
+        <f t="shared" si="0"/>
+        <v>0.12199999999999989</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>3.0981000000000001</v>
+      </c>
+      <c r="C9">
+        <v>2.9417</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.15640000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>3.0985999999999998</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2.9367000000000001</v>
       </c>
-      <c r="D9">
-        <f xml:space="preserve"> B9 - C9</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>0.16189999999999971</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data - half done (36 of 72 images)
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Smith\Desktop\MiTech Backup\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97269D69-A225-4485-B70F-FCAE773CFA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA0F8CE-3FB7-4CD7-A33E-7F23425C730D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4430" yWindow="1810" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Power While Running</t>
   </si>
@@ -116,6 +116,42 @@
   </si>
   <si>
     <t>Peter_Jamieson_2015_double_png_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_full_bmp_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_full_bmp_remote_to_local_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_full_png_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_full_png_remote_to_local_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_half_bmp_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_half_bmp_remote_to_local_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_half_png_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Peter_Jamieson_2015_half_png_remote_to_local_from_PI</t>
+  </si>
+  <si>
+    <t>Redhawk_logo_Double_bmp_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Redhawk_Logo_double_bmp_remote_to_local_from_PI</t>
+  </si>
+  <si>
+    <t>Redhawk_logo_Double_png_local_to_remote_from_PI</t>
+  </si>
+  <si>
+    <t>Redhawk_Logo_double_png_remote_to_local_from_PI</t>
   </si>
 </sst>
 </file>
@@ -442,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,7 +697,7 @@
         <v>2.9518</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D25" si="1" xml:space="preserve"> B14 - C14</f>
+        <f t="shared" ref="D14:D37" si="1" xml:space="preserve"> B14 - C14</f>
         <v>0.15079999999999982</v>
       </c>
     </row>
@@ -828,6 +864,186 @@
       <c r="D25">
         <f t="shared" si="1"/>
         <v>7.1299999999999919E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>3.0295999999999998</v>
+      </c>
+      <c r="C26">
+        <v>2.9251</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>0.10449999999999982</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>2.9967000000000001</v>
+      </c>
+      <c r="C27">
+        <v>2.8813</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0.11540000000000017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>2.9607999999999999</v>
+      </c>
+      <c r="C28">
+        <v>2.8071999999999999</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.15359999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>2.911</v>
+      </c>
+      <c r="C29">
+        <v>2.8113999999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>9.9600000000000133E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>2.9196</v>
+      </c>
+      <c r="C30">
+        <v>2.8525</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>6.7099999999999937E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>2.8927</v>
+      </c>
+      <c r="C31">
+        <v>2.7452000000000001</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0.14749999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>2.8736000000000002</v>
+      </c>
+      <c r="C32">
+        <v>2.8094999999999999</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>6.4100000000000268E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>2.8765999999999998</v>
+      </c>
+      <c r="C33">
+        <v>2.8129</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>6.3699999999999868E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>3.1065</v>
+      </c>
+      <c r="C34">
+        <v>3.0320999999999998</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>7.4400000000000244E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>3.1074000000000002</v>
+      </c>
+      <c r="C35">
+        <v>3.0314999999999999</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>7.5900000000000301E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>2.9175</v>
+      </c>
+      <c r="C36">
+        <v>2.8414000000000001</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>7.6099999999999834E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>2.8730000000000002</v>
+      </c>
+      <c r="C37">
+        <v>2.7812999999999999</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>9.1700000000000337E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
putting in this one data I did before my laptop kills me
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smith367\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Smith\Desktop\MiTech Backup\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA9D55D-3D89-498A-BC5E-C4382873A194}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4216B71-EC13-4BB4-A7A1-7CCA23B98169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1815" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4430" yWindow="1810" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Power While Running</t>
   </si>
@@ -181,6 +191,9 @@
   </si>
   <si>
     <t>PC_Local_to_PI_Peter_Jamieson_half_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Peter_Jamieson_half_png</t>
   </si>
 </sst>
 </file>
@@ -509,19 +522,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="52.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -535,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -550,7 +563,7 @@
         <v>5.1499999999999879E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -565,7 +578,7 @@
         <v>7.0399999999999796E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -580,7 +593,7 @@
         <v>6.5799999999999859E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -595,7 +608,7 @@
         <v>8.1999999999999851E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -610,7 +623,7 @@
         <v>6.490000000000018E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -625,7 +638,7 @@
         <v>5.7700000000000085E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -640,7 +653,7 @@
         <v>3.8200000000000234E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -655,7 +668,7 @@
         <v>6.2300000000000022E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -670,7 +683,7 @@
         <v>6.8499999999999783E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -685,7 +698,7 @@
         <v>5.7199999999999918E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -700,7 +713,7 @@
         <v>5.2500000000000213E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -715,7 +728,7 @@
         <v>3.819999999999979E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -726,11 +739,11 @@
         <v>2.9518</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D44" si="1" xml:space="preserve"> B14 - C14</f>
+        <f t="shared" ref="D14:D39" si="1" xml:space="preserve"> B14 - C14</f>
         <v>0.15079999999999982</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -745,7 +758,7 @@
         <v>0.1503000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,7 +773,7 @@
         <v>0.13419999999999987</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -775,7 +788,7 @@
         <v>0.16159999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -790,7 +803,7 @@
         <v>0.12199999999999989</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -805,7 +818,7 @@
         <v>0.15640000000000009</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -820,7 +833,7 @@
         <v>0.16189999999999971</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -835,7 +848,7 @@
         <v>8.8199999999999612E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -850,7 +863,7 @@
         <v>8.1500000000000128E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -865,7 +878,7 @@
         <v>5.1400000000000112E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -880,7 +893,7 @@
         <v>7.9900000000000304E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -895,7 +908,7 @@
         <v>7.1299999999999919E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -910,7 +923,7 @@
         <v>0.10449999999999982</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -925,7 +938,7 @@
         <v>0.11540000000000017</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -940,7 +953,7 @@
         <v>0.15359999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -955,7 +968,7 @@
         <v>9.9600000000000133E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -970,7 +983,7 @@
         <v>6.7099999999999937E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -985,7 +998,7 @@
         <v>0.14749999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1000,7 +1013,7 @@
         <v>6.4100000000000268E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1015,7 +1028,7 @@
         <v>6.3699999999999868E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -1030,7 +1043,7 @@
         <v>0.10280000000000022</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
@@ -1045,7 +1058,7 @@
         <v>0.11759999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1060,7 +1073,7 @@
         <v>0.12799999999999967</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1075,7 +1088,7 @@
         <v>0.17689999999999984</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -1090,7 +1103,22 @@
         <v>0.18820000000000014</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>3.5703999999999998</v>
+      </c>
+      <c r="C39">
+        <v>3.3765000000000001</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>0.19389999999999974</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -1101,11 +1129,11 @@
         <v>3.0320999999999998</v>
       </c>
       <c r="D46">
-        <f xml:space="preserve"> B46 - C46</f>
+        <f t="shared" ref="D46:D57" si="2" xml:space="preserve"> B46 - C46</f>
         <v>7.4400000000000244E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>36</v>
       </c>
@@ -1116,11 +1144,11 @@
         <v>3.0314999999999999</v>
       </c>
       <c r="D47">
-        <f xml:space="preserve"> B47 - C47</f>
+        <f t="shared" si="2"/>
         <v>7.5900000000000301E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>37</v>
       </c>
@@ -1131,11 +1159,11 @@
         <v>2.8414000000000001</v>
       </c>
       <c r="D48">
-        <f xml:space="preserve"> B48 - C48</f>
+        <f t="shared" si="2"/>
         <v>7.6099999999999834E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1146,11 +1174,11 @@
         <v>2.7812999999999999</v>
       </c>
       <c r="D49">
-        <f xml:space="preserve"> B49 - C49</f>
+        <f t="shared" si="2"/>
         <v>9.1700000000000337E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
@@ -1161,11 +1189,11 @@
         <v>2.8835000000000002</v>
       </c>
       <c r="D50">
-        <f xml:space="preserve"> B50 - C50</f>
+        <f t="shared" si="2"/>
         <v>7.8599999999999781E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
@@ -1176,11 +1204,11 @@
         <v>2.8704000000000001</v>
       </c>
       <c r="D51">
-        <f xml:space="preserve"> B51 - C51</f>
+        <f t="shared" si="2"/>
         <v>6.9799999999999862E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
@@ -1191,11 +1219,11 @@
         <v>2.7587999999999999</v>
       </c>
       <c r="D52">
-        <f xml:space="preserve"> B52 - C52</f>
+        <f t="shared" si="2"/>
         <v>4.8700000000000188E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>42</v>
       </c>
@@ -1206,11 +1234,11 @@
         <v>2.7521</v>
       </c>
       <c r="D53">
-        <f xml:space="preserve"> B53 - C53</f>
+        <f t="shared" si="2"/>
         <v>3.5899999999999821E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>43</v>
       </c>
@@ -1221,11 +1249,11 @@
         <v>2.7923</v>
       </c>
       <c r="D54">
-        <f xml:space="preserve"> B54 - C54</f>
+        <f t="shared" si="2"/>
         <v>8.3000000000000185E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
@@ -1236,11 +1264,11 @@
         <v>2.7713000000000001</v>
       </c>
       <c r="D55">
-        <f xml:space="preserve"> B55 - C55</f>
+        <f t="shared" si="2"/>
         <v>7.2699999999999765E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
@@ -1251,11 +1279,11 @@
         <v>2.7867999999999999</v>
       </c>
       <c r="D56">
-        <f xml:space="preserve"> B56 - C56</f>
+        <f t="shared" si="2"/>
         <v>4.8900000000000166E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
@@ -1266,7 +1294,7 @@
         <v>2.7505999999999999</v>
       </c>
       <c r="D57">
-        <f xml:space="preserve"> B57 - C57</f>
+        <f t="shared" si="2"/>
         <v>4.4599999999999973E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last of the Image data that I have
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Smith\Desktop\MiTech Backup\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4216B71-EC13-4BB4-A7A1-7CCA23B98169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E092282A-CAFA-4C74-A961-5BA8FBBB3CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4430" yWindow="1810" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Power While Running</t>
   </si>
@@ -194,6 +194,60 @@
   </si>
   <si>
     <t>PC_Local_to_PI_Peter_Jamieson_half_png</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_double_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_double_png</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_full_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_full_png</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_half_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_PI_Redhawk_Logo_half_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_Double_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_Double_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_full_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_full_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_half_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Peter_Jamieson_half_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_double_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_double_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_full_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_full_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_half_bmp</t>
+  </si>
+  <si>
+    <t>PC_Remote_from_PI_Redhawk_Logo_half_png</t>
   </si>
 </sst>
 </file>
@@ -520,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,7 +793,7 @@
         <v>2.9518</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D39" si="1" xml:space="preserve"> B14 - C14</f>
+        <f t="shared" ref="D14:D45" si="1" xml:space="preserve"> B14 - C14</f>
         <v>0.15079999999999982</v>
       </c>
     </row>
@@ -1118,6 +1172,96 @@
         <v>0.19389999999999974</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40">
+        <v>3.6937000000000002</v>
+      </c>
+      <c r="C40">
+        <v>3.6193</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>7.4400000000000244E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41">
+        <v>3.6280999999999999</v>
+      </c>
+      <c r="C41">
+        <v>3.53</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>9.8100000000000076E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <v>3.6173000000000002</v>
+      </c>
+      <c r="C42">
+        <v>3.5207999999999999</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>9.6500000000000252E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43">
+        <v>3.5758000000000001</v>
+      </c>
+      <c r="C43">
+        <v>3.4148000000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>0.16100000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44">
+        <v>3.5489000000000002</v>
+      </c>
+      <c r="C44">
+        <v>3.3898999999999999</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>0.15900000000000025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45">
+        <v>3.5731999999999999</v>
+      </c>
+      <c r="C45">
+        <v>3.3988</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>0.17439999999999989</v>
+      </c>
+    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>35</v>
@@ -1129,7 +1273,7 @@
         <v>3.0320999999999998</v>
       </c>
       <c r="D46">
-        <f t="shared" ref="D46:D57" si="2" xml:space="preserve"> B46 - C46</f>
+        <f t="shared" ref="D46:D69" si="2" xml:space="preserve"> B46 - C46</f>
         <v>7.4400000000000244E-2</v>
       </c>
     </row>
@@ -1296,6 +1440,186 @@
       <c r="D57">
         <f t="shared" si="2"/>
         <v>4.4599999999999973E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58">
+        <v>3.6657000000000002</v>
+      </c>
+      <c r="C58">
+        <v>3.5434999999999999</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>0.12220000000000031</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59">
+        <v>3.5545</v>
+      </c>
+      <c r="C59">
+        <v>3.3877000000000002</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>0.16679999999999984</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60">
+        <v>3.5705</v>
+      </c>
+      <c r="C60">
+        <v>3.4542999999999999</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>0.11620000000000008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61">
+        <v>3.5394999999999999</v>
+      </c>
+      <c r="C61">
+        <v>3.3852000000000002</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>0.15429999999999966</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62">
+        <v>3.5924999999999998</v>
+      </c>
+      <c r="C62">
+        <v>3.4386999999999999</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>0.15379999999999994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63">
+        <v>3.5672999999999999</v>
+      </c>
+      <c r="C63">
+        <v>3.3717000000000001</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>0.19559999999999977</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>3.6579000000000002</v>
+      </c>
+      <c r="C64">
+        <v>3.5529000000000002</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>0.10499999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>3.5653000000000001</v>
+      </c>
+      <c r="C65">
+        <v>3.3624000000000001</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>0.20290000000000008</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>3.5749</v>
+      </c>
+      <c r="C66">
+        <v>3.3887999999999998</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>0.18610000000000015</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>3.5333000000000001</v>
+      </c>
+      <c r="C67">
+        <v>3.3940999999999999</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>0.13920000000000021</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>3.5323000000000002</v>
+      </c>
+      <c r="C68">
+        <v>3.3715000000000002</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>0.16080000000000005</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>3.5270000000000001</v>
+      </c>
+      <c r="C69">
+        <v>3.3954</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>0.13160000000000016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on Naming Conventions
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBSwi\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34DE8D3-39B7-4C4B-9A5F-66185BEB9C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900848C2-E980-4D9A-A5CD-F8BA608089C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Naming Conventions" sheetId="2" r:id="rId1"/>
     <sheet name="Results" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>Power While Running</t>
   </si>
@@ -312,6 +313,30 @@
   </si>
   <si>
     <t>*Remote PC in all tests was a Ubuntu 20.04LTS virtual machine running in Vmware Workstation with ethernet adapter passed through.</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_full_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_Double_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_half_bmp</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_half_png</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_Double_png</t>
+  </si>
+  <si>
+    <t>PC_Local_to_Remote_MiamiM_full_png</t>
+  </si>
+  <si>
+    <t>PC_Remote_to_Local_MiamiM_full_png</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_full_PNG</t>
   </si>
 </sst>
 </file>
@@ -650,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7039B93-5E26-40BD-BA88-891EC33FC8BB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -718,1175 +743,1409 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="52.47265625" customWidth="1"/>
-    <col min="2" max="2" width="18.7890625" customWidth="1"/>
-    <col min="3" max="3" width="22.15625" customWidth="1"/>
-    <col min="4" max="4" width="13.15625" customWidth="1"/>
+    <col min="1" max="2" width="52.47265625" customWidth="1"/>
+    <col min="3" max="3" width="18.7890625" customWidth="1"/>
+    <col min="4" max="4" width="22.15625" customWidth="1"/>
+    <col min="5" max="5" width="13.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2">
         <v>2.8271999999999999</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2.7757000000000001</v>
       </c>
-      <c r="D2">
-        <f xml:space="preserve"> B2-C2</f>
+      <c r="E2">
+        <f xml:space="preserve"> C2-D2</f>
         <v>5.1499999999999879E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
         <v>2.8386999999999998</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2.7683</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D13" si="0" xml:space="preserve"> B3 - C3</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="0" xml:space="preserve"> C3 - D3</f>
         <v>7.0399999999999796E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
         <v>2.8666</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2.8008000000000002</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>6.5799999999999859E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
         <v>2.8900999999999999</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2.8081</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>8.1999999999999851E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
         <v>2.8603000000000001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2.7953999999999999</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>6.490000000000018E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>2.8353999999999999</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2.7776999999999998</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>5.7700000000000085E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
         <v>2.8203</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2.7820999999999998</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>3.8200000000000234E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
         <v>2.8147000000000002</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2.7524000000000002</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>6.2300000000000022E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
         <v>2.8296999999999999</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>2.7612000000000001</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>6.8499999999999783E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
         <v>2.8022999999999998</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2.7450999999999999</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>5.7199999999999918E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
         <v>2.7978000000000001</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2.7452999999999999</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>5.2500000000000213E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
         <v>2.7907999999999999</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2.7526000000000002</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>3.819999999999979E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14">
         <v>3.1025999999999998</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2.9518</v>
       </c>
-      <c r="D14">
-        <f t="shared" ref="D14:D45" si="1" xml:space="preserve"> B14 - C14</f>
+      <c r="E14">
+        <f t="shared" ref="E14:E45" si="1" xml:space="preserve"> C14 - D14</f>
         <v>0.15079999999999982</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15">
         <v>3.0836000000000001</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>2.9333</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="1"/>
         <v>0.1503000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
         <v>3.0442</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2.91</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="1"/>
         <v>0.13419999999999987</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17">
         <v>3.0968</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>2.9352</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="1"/>
         <v>0.16159999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18">
         <v>3.0960000000000001</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>2.9740000000000002</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <f t="shared" si="1"/>
         <v>0.12199999999999989</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19">
         <v>3.0981000000000001</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>2.9417</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f t="shared" si="1"/>
         <v>0.15640000000000009</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20">
         <v>3.0985999999999998</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>2.9367000000000001</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <f t="shared" si="1"/>
         <v>0.16189999999999971</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
         <v>3.0301999999999998</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>2.9420000000000002</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <f t="shared" si="1"/>
         <v>8.8199999999999612E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
         <v>3.0945</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>3.0129999999999999</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <f t="shared" si="1"/>
         <v>8.1500000000000128E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
         <v>3.1352000000000002</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>3.0838000000000001</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <f t="shared" si="1"/>
         <v>5.1400000000000112E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
         <v>3.0554000000000001</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>2.9754999999999998</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <f t="shared" si="1"/>
         <v>7.9900000000000304E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
         <v>3.0956000000000001</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>3.0243000000000002</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <f t="shared" si="1"/>
         <v>7.1299999999999919E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
         <v>3.0295999999999998</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>2.9251</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <f t="shared" si="1"/>
         <v>0.10449999999999982</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
         <v>2.9967000000000001</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>2.8813</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <f t="shared" si="1"/>
         <v>0.11540000000000017</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
         <v>2.9607999999999999</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>2.8071999999999999</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <f t="shared" si="1"/>
         <v>0.15359999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
         <v>2.911</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>2.8113999999999999</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <f t="shared" si="1"/>
         <v>9.9600000000000133E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
         <v>2.9196</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>2.8525</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <f t="shared" si="1"/>
         <v>6.7099999999999937E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
         <v>2.8927</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>2.7452000000000001</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <f t="shared" si="1"/>
         <v>0.14749999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
         <v>2.8736000000000002</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>2.8094999999999999</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <f t="shared" si="1"/>
         <v>6.4100000000000268E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
         <v>2.8765999999999998</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>2.8129</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <f t="shared" si="1"/>
         <v>6.3699999999999868E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34">
         <v>3.681</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>3.5781999999999998</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <f t="shared" si="1"/>
         <v>0.10280000000000022</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35">
         <v>3.6078000000000001</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>3.4902000000000002</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <f t="shared" si="1"/>
         <v>0.11759999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36">
         <v>3.5861999999999998</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>3.4582000000000002</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <f t="shared" si="1"/>
         <v>0.12799999999999967</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
         <v>3.5468999999999999</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>3.37</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <f t="shared" si="1"/>
         <v>0.17689999999999984</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38">
         <v>3.5493000000000001</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>3.3611</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <f t="shared" si="1"/>
         <v>0.18820000000000014</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39">
         <v>3.5703999999999998</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>3.3765000000000001</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <f t="shared" si="1"/>
         <v>0.19389999999999974</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40">
         <v>3.6937000000000002</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>3.6193</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <f t="shared" si="1"/>
         <v>7.4400000000000244E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41">
         <v>3.6280999999999999</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>3.53</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <f t="shared" si="1"/>
         <v>9.8100000000000076E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42">
         <v>3.6173000000000002</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>3.5207999999999999</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <f t="shared" si="1"/>
         <v>9.6500000000000252E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43">
         <v>3.5758000000000001</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>3.4148000000000001</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <f t="shared" si="1"/>
         <v>0.16100000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44">
         <v>3.5489000000000002</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>3.3898999999999999</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <f t="shared" si="1"/>
         <v>0.15900000000000025</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45">
         <v>3.5731999999999999</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>3.3988</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <f t="shared" si="1"/>
         <v>0.17439999999999989</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46">
         <v>3.1065</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>3.0320999999999998</v>
       </c>
-      <c r="D46">
-        <f t="shared" ref="D46:D69" si="2" xml:space="preserve"> B46 - C46</f>
+      <c r="E46">
+        <f t="shared" ref="E46:E69" si="2" xml:space="preserve"> C46 - D46</f>
         <v>7.4400000000000244E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47">
         <v>3.1074000000000002</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>3.0314999999999999</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <f t="shared" si="2"/>
         <v>7.5900000000000301E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48">
         <v>2.9175</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>2.8414000000000001</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <f t="shared" si="2"/>
         <v>7.6099999999999834E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49">
         <v>2.8730000000000002</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>2.7812999999999999</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <f t="shared" si="2"/>
         <v>9.1700000000000337E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50">
         <v>2.9621</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>2.8835000000000002</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <f t="shared" si="2"/>
         <v>7.8599999999999781E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51">
         <v>2.9401999999999999</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>2.8704000000000001</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <f t="shared" si="2"/>
         <v>6.9799999999999862E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52">
         <v>2.8075000000000001</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>2.7587999999999999</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <f t="shared" si="2"/>
         <v>4.8700000000000188E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53">
         <v>2.7879999999999998</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>2.7521</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <f t="shared" si="2"/>
         <v>3.5899999999999821E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54">
         <v>2.8753000000000002</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>2.7923</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <f t="shared" si="2"/>
         <v>8.3000000000000185E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55">
         <v>2.8439999999999999</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>2.7713000000000001</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <f t="shared" si="2"/>
         <v>7.2699999999999765E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56">
         <v>2.8357000000000001</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>2.7867999999999999</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <f t="shared" si="2"/>
         <v>4.8900000000000166E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57">
         <v>2.7951999999999999</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>2.7505999999999999</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <f t="shared" si="2"/>
         <v>4.4599999999999973E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58">
         <v>3.6657000000000002</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>3.5434999999999999</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <f t="shared" si="2"/>
         <v>0.12220000000000031</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59">
         <v>3.5545</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>3.3877000000000002</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <f t="shared" si="2"/>
         <v>0.16679999999999984</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60">
         <v>3.5705</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>3.4542999999999999</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <f t="shared" si="2"/>
         <v>0.11620000000000008</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61">
         <v>3.5394999999999999</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>3.3852000000000002</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <f t="shared" si="2"/>
         <v>0.15429999999999966</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62">
         <v>3.5924999999999998</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>3.4386999999999999</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <f t="shared" si="2"/>
         <v>0.15379999999999994</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63">
         <v>3.5672999999999999</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>3.3717000000000001</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <f t="shared" si="2"/>
         <v>0.19559999999999977</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
         <v>3.6579000000000002</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>3.5529000000000002</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <f t="shared" si="2"/>
         <v>0.10499999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65">
         <v>3.5653000000000001</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>3.3624000000000001</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <f t="shared" si="2"/>
         <v>0.20290000000000008</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66">
         <v>3.5749</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>3.3887999999999998</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <f t="shared" si="2"/>
         <v>0.18610000000000015</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
         <v>3.5333000000000001</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>3.3940999999999999</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <f t="shared" si="2"/>
         <v>0.13920000000000021</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68">
         <v>3.5323000000000002</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>3.3715000000000002</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <f t="shared" si="2"/>
         <v>0.16080000000000005</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69">
         <v>3.5270000000000001</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>3.3954</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <f t="shared" si="2"/>
         <v>0.13160000000000016</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
         <v>3.7231000000000001</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>3.5756999999999999</v>
       </c>
-      <c r="D71">
-        <f xml:space="preserve"> B71-C71</f>
+      <c r="E71">
+        <f xml:space="preserve"> C71-D71</f>
         <v>0.1474000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
         <v>3.71</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>3.5897000000000001</v>
       </c>
-      <c r="D72">
-        <f t="shared" ref="D72:D78" si="3">B72-C72</f>
+      <c r="E72">
+        <f t="shared" ref="E72:E78" si="3">C72-D72</f>
         <v>0.12029999999999985</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73">
         <v>3.6597</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>3.5615000000000001</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <f t="shared" si="3"/>
         <v>9.8199999999999843E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74">
         <v>3.7641</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>3.6469999999999998</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <f t="shared" si="3"/>
         <v>0.1171000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75">
         <v>3.7387999999999999</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>3.6238999999999999</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <f t="shared" si="3"/>
         <v>0.1149</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76">
         <v>3.7433000000000001</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>3.6680999999999999</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <f t="shared" si="3"/>
         <v>7.5200000000000156E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77">
         <v>3.6892</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>3.6126999999999998</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <f t="shared" si="3"/>
         <v>7.6500000000000234E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78">
         <v>3.8226</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>3.7582</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <f t="shared" si="3"/>
         <v>6.4400000000000013E-2</v>
       </c>

</xml_diff>

<commit_message>
Miami M files corrected
</commit_message>
<xml_diff>
--- a/Sqlite/File_Transfer_Test_Results.xlsx
+++ b/Sqlite/File_Transfer_Test_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBSwi\Documents\GitHub\Senior-Design-Project\Sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900848C2-E980-4D9A-A5CD-F8BA608089C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18757F5D-6BB3-4890-8E91-7D70671DF0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12156" yWindow="1872" windowWidth="17280" windowHeight="9174" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Naming Conventions" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
   <si>
     <t>Power While Running</t>
   </si>
@@ -337,6 +337,36 @@
   </si>
   <si>
     <t>PI_Remote_To_Local_MiamiM_full_PNG</t>
+  </si>
+  <si>
+    <t>PI_Local_To_Remote_MiamiM_full_bmp</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_full_BMP</t>
+  </si>
+  <si>
+    <t>PI_Local_To_Remote_MiamiM_Double_BMP</t>
+  </si>
+  <si>
+    <t>PI_Local_To_Remote_MiamiM_Double_PNG</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_Double_BMP</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_Double_PNG</t>
+  </si>
+  <si>
+    <t>PI_Local_To_Remote_MiamiM_Half_BMP</t>
+  </si>
+  <si>
+    <t>PI_Local_to_Remote_MiamiM_Half_PNG</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_Half_PNG</t>
+  </si>
+  <si>
+    <t>PI_Remote_To_Local_MiamiM_Half_BMP</t>
   </si>
 </sst>
 </file>
@@ -745,13 +775,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="52.47265625" customWidth="1"/>
+    <col min="1" max="1" width="5.7890625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="52.47265625" customWidth="1"/>
     <col min="3" max="3" width="18.7890625" customWidth="1"/>
     <col min="4" max="4" width="22.15625" customWidth="1"/>
     <col min="5" max="5" width="13.15625" customWidth="1"/>
@@ -815,7 +846,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>2.8666</v>
@@ -833,7 +864,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C5">
         <v>2.8900999999999999</v>
@@ -851,7 +882,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="C6">
         <v>2.8603000000000001</v>
@@ -869,7 +900,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="C7">
         <v>2.8353999999999999</v>
@@ -887,7 +918,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="C8">
         <v>2.8203</v>
@@ -905,7 +936,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>2.8147000000000002</v>
@@ -923,7 +954,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>2.8296999999999999</v>
@@ -941,7 +972,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>2.8022999999999998</v>
@@ -959,7 +990,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="C12">
         <v>2.7978000000000001</v>
@@ -977,7 +1008,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="C13">
         <v>2.7907999999999999</v>

</xml_diff>